<commit_message>
corrected typo and added a new chunk
</commit_message>
<xml_diff>
--- a/FRAME_Chia Wen+Mingqian.xlsx
+++ b/FRAME_Chia Wen+Mingqian.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\0. study abroad\academic\11. 2024 Winter\1. SurvMeth 745 Practical Tools for Study Design and Inference\2. Assignments\Project (Apr 1)\SurvMeth-745\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FAF367A-0B1D-456F-AB18-000BE5ABBF47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4C97892-84C7-4A73-8991-3C0709B92B90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4499,10 +4499,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:BD539"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AU1" zoomScale="96" workbookViewId="0">
-      <selection activeCell="BC7" sqref="BC7"/>
+      <selection activeCell="BA10" sqref="BA10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -91384,7 +91387,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup fitToHeight="0" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageMargins left="0.3" right="0.3" top="0.25" bottom="0.25" header="0.3" footer="0.3"/>
+  <pageSetup scale="16" fitToHeight="0" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>